<commit_message>
a lot of additions
</commit_message>
<xml_diff>
--- a/Project_TS_Log.xlsx
+++ b/Project_TS_Log.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\FlutterProjects\GitHUBRepos\Instagram-Clone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\FlutterProjects\instagram_clone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B89C335-C62E-46E6-A054-88AB299D00B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918D1ECD-3623-43D9-ADEC-AB60B4503139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3830" yWindow="2140" windowWidth="19200" windowHeight="10510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Day</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Added textInputFields and created loginScreen file and configured firebase.</t>
+  </si>
+  <si>
+    <t>Created authRepo, authController, firebase instance providers, utilities having imagePIcker and showSnackBar, created and worked on SignUpScreen and setup functions.</t>
   </si>
 </sst>
 </file>
@@ -392,7 +395,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -446,7 +449,18 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
+      <c r="A4" s="2">
+        <v>45223</v>
+      </c>
+      <c r="B4" s="3">
+        <v>67</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>

</xml_diff>

<commit_message>
Added bottom nav bar and add post
</commit_message>
<xml_diff>
--- a/Project_TS_Log.xlsx
+++ b/Project_TS_Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\FlutterProjects\instagram_clone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A6DA9F-767E-4295-AC1D-0E6844235837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C526D4F-FDAF-4267-A82E-08D9285E80C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4150" yWindow="3480" windowWidth="19200" windowHeight="10510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2640" yWindow="1040" windowWidth="15470" windowHeight="10510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Day</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Fixed bugs, added userProvider, changed project strucutre (total revamp) and finished persistent authentication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added postImage screen, setup backend for posts, tabBar. Created post model and started feed Screen work. </t>
   </si>
 </sst>
 </file>
@@ -403,8 +406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -514,7 +517,18 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
+      <c r="A8" s="5">
+        <v>45236</v>
+      </c>
+      <c r="B8" s="3">
+        <v>82</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="18" spans="1:4" s="4" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>